<commit_message>
Removed useless files, improved substitution test
</commit_message>
<xml_diff>
--- a/doc/or1200_sub_v3.xlsx
+++ b/doc/or1200_sub_v3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="173">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -37,9 +37,8 @@
     <t xml:space="preserve">l.add rD,rA,rB</t>
   </si>
   <si>
-    <t xml:space="preserve">l.addi r0,rA,0
-l.addc rD,r0,rB
-l.andi r0,r0,0</t>
+    <t xml:space="preserve">l.addi r0,r0,0
+l.addc rD,rA,rB</t>
   </si>
   <si>
     <t xml:space="preserve">l.add rD,rA,rB
@@ -58,44 +57,26 @@
   </si>
   <si>
     <t xml:space="preserve">l.addi rD,rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.addc r0,r0,r0
-l.addic rD,rA,I
-l.movhi r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,I
-l.add rD,rA,r0
-l.movhi r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.addic rD,rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,I
-l.addc rD,rA,r0
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.addic rD,rA,I
-l.and r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.and rD,rA,rB</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
         <rFont val="DejaVu Sans"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">l.xori r0,rA,-1
-l.xori rD,rB,-1
-l.or rD,</t>
+      <t xml:space="preserve">l.addic r0,r0,0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">l.movhi r0,0
+</t>
     </r>
     <r>
       <rPr>
@@ -104,7 +85,51 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">rD,r0
+      <t xml:space="preserve">l.addic rD,rA,I
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xori rD,rA,r0
+l.xori r0,r0,I
+l.add rD,rD,r0
+l.movhi r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.addic rD,rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xori r0,r0,I
+l.addc rD,rA,r0
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.addic rD,rA,I
+l.and r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.and rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.and rD,rA,rB
+l.extbs r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.and rD,rA,rB
+l.extbz r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.andi rD,rA,K</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">l.xori rD,rA,-1
 </t>
     </r>
     <r>
@@ -115,28 +140,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">l.xori rD,rD,-1
-l.xor r0,r0,r0</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">l.and rD,rA,rB
-l.extbs r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.andi rD,rA,K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.ori r0,r0,K
+      <t xml:space="preserve">l.ori r0,r0,K
 l.xori r0,r0,-1
-l.xori rD,rA,-1
 l.or rD,rD,r0
 l.xori rD,rD,-1
 l.xor r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.ori r0,r0,K
-l.and rD,rA,r0
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.ori r0,r0,K
+l.and rD,rD,r0
 l.xor r0,r0,r0</t>
   </si>
   <si>
@@ -360,6 +374,10 @@
   </si>
   <si>
     <t xml:space="preserve">l.movhi rD,K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.movhi rD,K
+l.xor r0,r0,r0</t>
   </si>
   <si>
     <t xml:space="preserve">l.ori rD,r0,K
@@ -411,6 +429,17 @@
   </si>
   <si>
     <t xml:space="preserve">l.or rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.or rD,rA,rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.or rD,rA,rB
+l.mulu r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.ori rD,rA,K</t>
   </si>
   <si>
     <r>
@@ -419,20 +448,8 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">l.xori r0,rA,-1
-l.xori rD,rB,-1
-l.and rD,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">rD,r0
+      <t xml:space="preserve">l.xori rD,rA,-1
 </t>
     </r>
     <r>
@@ -443,232 +460,24 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">l.xori rD,rD,-1
-l.xor r0, r0, r0</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">l.or rD,rA,rB
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.ori rD,rA,K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,K
+      <t xml:space="preserve">l.xori r0,r0,K
 l.xori r0,r0,-1
-l.xori rD,rA,-1
 l.and rD,rD,r0
 l.xori rD,rD,-1
 l.xor r0, r0, r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,K
-l.or rD,rA,r0
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.psync</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.rfe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.ror rD,rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.rori rD,rA,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,L
-l.xori r0,r0,31
-l.addi r0,r0,33
-l.sll r0,rA,r0
-l.srli rD,rA,L
-l.or rD,rD,r0
-l.xor r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.rori rD,rA,L
-l.and r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sb I(rA),rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sd I(rA),rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfeq rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfeqi rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfges rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgesi rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgeu rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgeui rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgts rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgtsi rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgtu rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfgtui rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfles rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sflesi rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfleu rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfleui rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sflts rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfltsi rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfltu rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfltui rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfne rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sfnei rA,I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sh I(rA),rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sh I(rA),rB
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sh I(rA),rB
-l.and r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sll rD,rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sll rD,rA,rB
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sll rD,rA,rB
-l.muli r0,r0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.slli rD,rA,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,I
-l.sll rD,rA,r0
-l.xor r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.slli rD,rA,L
-l.and r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sra rD,rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sra rD,rA,rB
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sra rD,rA,rB
-l.muli r0,r0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srai rD,rA,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,I
-l.sra rD,rA,r0
-l.xor r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srai rD,rA,L
-l.and r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srl rD,rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srl rD,rA,rB
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srl rD,rA,rB
-l.muli r0,r0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srli rD,rA,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori r0,r0,I
-l.srl rD,rA,r0
-l.xor r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.srli rD,rA,L
-l.and r0,r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sub rD,rA,rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sub rD,rA,rB
-l.extws r0,r0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sub rD,rA,rB
-l.xori r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sw I(rA),rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sw I(rA),rB
-l.andi r0,r0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.swa I(rA),rB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.sys K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.trap K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xor rD,rA,rB</t>
-  </si>
-  <si>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">l.xor rD,r0,rA
+l.xori r0,r0,K
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -676,32 +485,269 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">l.and r0,rA,rB
-l.xori r0, r0, -1
-l.or rD,rA,rB
-l.and rD,rD,r0
+      <t xml:space="preserve">l.or rD,rA,r0
+l.andi r0,r0,0</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">l.psync</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.rfe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.ror rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.ror rD,rA,rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.ror rD,rA,rB
+l.movhi r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.rori rD,rA,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.xori r0,r0,L
+l.xori r0,r0,31
+l.addi r0,r0,33
+l.sll r0,rD,r0
+l.srli rD,rD,L
+l.or rD,rD,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.rori rD,rA,L
+l.and r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sb I(rA),rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sd I(rA),rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfeq rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfeqi rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfges rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgesi rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgeu rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgeui rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgts rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgtsi rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgtu rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfgtui rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfles rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sflesi rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfleu rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfleui rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sflts rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfltsi rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfltu rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfltui rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfne rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sfnei rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sh I(rA),rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sh I(rA),rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sh I(rA),rB
+l.and r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sll rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sll rD,rA,rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sll rD,rA,rB
+l.muli r0,r0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.slli rD,rA,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.xori r0,r0,I
+l.sll rD,rA,r0
+l.xor r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.slli rD,rA,L
+l.and r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sra rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sra rD,rA,rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sra rD,rA,rB
+l.muli r0,r0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srai rD,rA,L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">l.xor rD,rA,r0
 </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
         <rFont val="DejaVu Sans"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">l.xor r0, r0, r0</t>
+      <t xml:space="preserve">l.xori r0,r0,I
+l.sra rD,rA,r0
+l.xor r0,r0,r0</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srai rD,rA,L
+l.and r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srl rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srl rD,rA,rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srl rD,rA,rB
+l.muli r0,r0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srli rD,rA,L</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">l.xor rD,rA,r0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">l.xori r0,r0,I
+l.srl rD,rA,r0
+l.xor r0,r0,r0</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">l.srli rD,rA,L
+l.and r0,r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sub rD,rA,rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sub rD,rA,rB
+l.extws r0,r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sub rD,rA,rB
+l.xori r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sw I(rA),rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sw I(rA),rB
+l.andi r0,r0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.swa I(rA),rB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.sys K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.trap K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xor rD,rA,rB</t>
   </si>
   <si>
     <t xml:space="preserve">l.xor rD,rA,rB
 l.rori r0,r0,0</t>
   </si>
   <si>
+    <t xml:space="preserve">l.xor rD,rA,rB
+l.slli r0,r0,0</t>
+  </si>
+  <si>
     <t xml:space="preserve">l.xori rD,rA,I</t>
   </si>
   <si>
-    <t xml:space="preserve">l.ori r0,r0,I
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.ori r0,r0,I
 l.xor rD,rA,r0
 l.andi r0,r0,0</t>
   </si>
@@ -717,7 +763,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
@@ -737,6 +783,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
       <family val="0"/>
     </font>
     <font>
@@ -813,7 +870,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -842,7 +899,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -856,6 +913,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -937,8 +1002,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -972,7 +1037,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1062,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1027,11 +1092,11 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1423,7 +1488,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -1433,7 +1498,9 @@
       <c r="C46" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -1441,7 +1508,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1450,7 +1517,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1459,7 +1526,7 @@
     </row>
     <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1469,19 +1536,19 @@
     </row>
     <row r="50" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1490,7 +1557,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1499,7 +1566,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1508,7 +1575,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -1516,7 +1583,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1524,39 +1591,39 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="B57" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="C57" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" s="5" t="s">
         <v>106</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="3"/>
@@ -1564,38 +1631,42 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1603,7 +1674,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -1611,7 +1682,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1619,14 +1690,14 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B67" s="3"/>
       <c r="D67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1634,7 +1705,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -1642,7 +1713,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1650,13 +1721,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1664,13 +1735,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1679,7 +1750,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -1687,7 +1758,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1695,14 +1766,14 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B77" s="3"/>
       <c r="D77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1710,13 +1781,13 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1724,14 +1795,14 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B81" s="3"/>
       <c r="D81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1739,7 +1810,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
@@ -1747,7 +1818,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1755,86 +1826,86 @@
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D86" s="5"/>
     </row>
-    <row r="87" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="5"/>
@@ -1842,31 +1913,31 @@
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -1874,35 +1945,35 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D97" s="5"/>
     </row>
-    <row r="98" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More reliable branch behavior
</commit_message>
<xml_diff>
--- a/doc/or1200_sub_v3.xlsx
+++ b/doc/or1200_sub_v3.xlsx
@@ -59,38 +59,11 @@
     <t xml:space="preserve">l.addi rD,rA,I</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.addic r0,r0,0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">l.movhi r0,0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.addic rD,rA,I
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">l.xori rD,rA,r0
+    <t xml:space="preserve">l.add r0,r0,r0
+l.addic rD,rA,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l.xor rD,rA,r0
 l.xori r0,r0,I
 l.add rD,rD,r0
 l.movhi r0,0</t>
@@ -99,8 +72,9 @@
     <t xml:space="preserve">l.addic rD,rA,I</t>
   </si>
   <si>
-    <t xml:space="preserve">l.xori r0,r0,I
-l.addc rD,rA,r0
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.xori r0,r0,I
+l.addc rD,rD,r0
 l.andi r0,r0,0</t>
   </si>
   <si>
@@ -122,30 +96,12 @@
     <t xml:space="preserve">l.andi rD,rA,K</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">l.xori rD,rA,-1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.ori r0,r0,K
+    <t xml:space="preserve">l.xori rD,rA,-1
+l.ori r0,r0,K
 l.xori r0,r0,-1
 l.or rD,rD,r0
 l.xori rD,rD,-1
 l.xor r0,r0,r0</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">l.xor rD,rA,r0
@@ -442,52 +398,18 @@
     <t xml:space="preserve">l.ori rD,rA,K</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">l.xori rD,rA,-1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.xori r0,r0,K
+    <t xml:space="preserve">l.xori rD,rA,-1
+l.xori r0,r0,K
 l.xori r0,r0,-1
 l.and rD,rD,r0
 l.xori rD,rD,-1
 l.xor r0, r0, r0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">l.xor rD,r0,rA
+  </si>
+  <si>
+    <t xml:space="preserve">l.xor rD,rA,r0
 l.xori r0,r0,K
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.or rD,rA,r0
+l.or rD,rA,r0
 l.andi r0,r0,0</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">l.psync</t>
@@ -617,7 +539,7 @@
   <si>
     <t xml:space="preserve">l.xor rD,rA,r0
 l.xori r0,r0,I
-l.sll rD,rA,r0
+l.sll rD,rD,r0
 l.xor r0,r0,r0</t>
   </si>
   <si>
@@ -639,26 +561,10 @@
     <t xml:space="preserve">l.srai rD,rA,L</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">l.xor rD,rA,r0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.xori r0,r0,I
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.xori r0,r0,I
 l.sra rD,rA,r0
 l.xor r0,r0,r0</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">l.srai rD,rA,L
@@ -679,26 +585,10 @@
     <t xml:space="preserve">l.srli rD,rA,L</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">l.xor rD,rA,r0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l.xori r0,r0,I
+    <t xml:space="preserve">l.xor rD,rA,r0
+l.xori r0,r0,I
 l.srl rD,rA,r0
 l.xor r0,r0,r0</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">l.srli rD,rA,L
@@ -748,7 +638,7 @@
   <si>
     <t xml:space="preserve">l.xor rD,rA,r0
 l.ori r0,r0,I
-l.xor rD,rA,r0
+l.xor rD,rD,r0
 l.andi r0,r0,0</t>
   </si>
   <si>
@@ -763,7 +653,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
@@ -787,24 +677,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="DejaVu Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,6 +698,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF58220"/>
+        <bgColor rgb="FFFF7F00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
@@ -826,7 +711,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7F00"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFF58220"/>
       </patternFill>
     </fill>
     <fill>
@@ -870,7 +755,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -891,36 +776,40 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -978,7 +867,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFF58220"/>
       <rgbColor rgb="FFFF7F00"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -1002,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B61" activeCellId="0" sqref="B61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1047,7 +936,7 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -1069,28 +958,28 @@
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1102,43 +991,43 @@
       <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="3"/>
@@ -1147,7 +1036,7 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="3"/>
@@ -1156,7 +1045,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="3"/>
@@ -1165,7 +1054,7 @@
       <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3"/>
@@ -1174,7 +1063,7 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="3"/>
@@ -1183,7 +1072,7 @@
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="3"/>
@@ -1192,7 +1081,7 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="3"/>
@@ -1201,7 +1090,7 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="3"/>
@@ -1210,7 +1099,7 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="3"/>
@@ -1219,7 +1108,7 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="3"/>
@@ -1228,7 +1117,7 @@
       <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="3"/>
@@ -1240,7 +1129,7 @@
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1253,20 +1142,20 @@
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1282,7 +1171,7 @@
       <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="3"/>
@@ -1338,24 +1227,24 @@
       <c r="E29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1363,13 +1252,13 @@
       <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1377,16 +1266,16 @@
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="3"/>
@@ -1397,25 +1286,25 @@
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1430,11 +1319,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -1443,7 +1332,7 @@
       <c r="D40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="3"/>
@@ -1452,7 +1341,7 @@
       <c r="E41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B42" s="3"/>
@@ -1461,7 +1350,7 @@
       <c r="E42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="3"/>
@@ -1470,18 +1359,18 @@
       <c r="E43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1492,22 +1381,22 @@
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B47" s="3"/>
@@ -1516,7 +1405,7 @@
       <c r="E47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B48" s="3"/>
@@ -1525,7 +1414,7 @@
       <c r="E48" s="3"/>
     </row>
     <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="11" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="3"/>
@@ -1547,7 +1436,7 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B51" s="3"/>
@@ -1556,7 +1445,7 @@
       <c r="E51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B52" s="3"/>
@@ -1565,24 +1454,24 @@
       <c r="E52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="11" t="s">
         <v>98</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="10"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3"/>
@@ -1593,7 +1482,7 @@
       <c r="A56" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D56" s="5"/>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -1605,32 +1494,32 @@
       <c r="C57" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="5"/>
+      <c r="B59" s="7"/>
       <c r="C59" s="3"/>
       <c r="E59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="10" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="3"/>
@@ -1651,7 +1540,7 @@
       <c r="A62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="7" t="s">
         <v>114</v>
       </c>
       <c r="C62" s="6" t="s">
@@ -1665,7 +1554,7 @@
       <c r="D63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B64" s="3"/>
@@ -1673,15 +1562,15 @@
       <c r="E64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
       <c r="D65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="10" t="s">
         <v>119</v>
       </c>
       <c r="B66" s="3"/>
@@ -1689,14 +1578,14 @@
       <c r="E66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="10" t="s">
         <v>120</v>
       </c>
       <c r="B67" s="3"/>
       <c r="D67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="10" t="s">
         <v>121</v>
       </c>
       <c r="B68" s="3"/>
@@ -1704,15 +1593,15 @@
       <c r="E68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
       <c r="D69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="10" t="s">
         <v>123</v>
       </c>
       <c r="B70" s="3"/>
@@ -1720,13 +1609,13 @@
       <c r="E70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="10" t="s">
         <v>124</v>
       </c>
       <c r="D71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="10" t="s">
         <v>125</v>
       </c>
       <c r="B72" s="3"/>
@@ -1734,13 +1623,13 @@
       <c r="E72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="10" t="s">
         <v>126</v>
       </c>
       <c r="D73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="10" t="s">
         <v>127</v>
       </c>
       <c r="B74" s="3"/>
@@ -1749,7 +1638,7 @@
       <c r="E74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="10" t="s">
         <v>128</v>
       </c>
       <c r="C75" s="3"/>
@@ -1757,7 +1646,7 @@
       <c r="E75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B76" s="3"/>
@@ -1765,14 +1654,14 @@
       <c r="E76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="10" t="s">
         <v>130</v>
       </c>
       <c r="B77" s="3"/>
       <c r="D77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="10" t="s">
         <v>131</v>
       </c>
       <c r="B78" s="3"/>
@@ -1780,13 +1669,13 @@
       <c r="E78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="10" t="s">
         <v>132</v>
       </c>
       <c r="D79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="10" t="s">
         <v>133</v>
       </c>
       <c r="B80" s="3"/>
@@ -1794,14 +1683,14 @@
       <c r="E80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="10" t="s">
         <v>134</v>
       </c>
       <c r="B81" s="3"/>
       <c r="D81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B82" s="3"/>
@@ -1809,15 +1698,15 @@
       <c r="E82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
       <c r="D83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="10" t="s">
         <v>137</v>
       </c>
       <c r="B84" s="3"/>
@@ -1828,10 +1717,10 @@
       <c r="A85" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="7" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1845,20 +1734,20 @@
       <c r="C86" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D86" s="5"/>
+      <c r="D86" s="7"/>
     </row>
     <row r="87" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="7" t="s">
         <v>145</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
@@ -1870,20 +1759,20 @@
       <c r="C88" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D88" s="5"/>
+      <c r="D88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
@@ -1895,21 +1784,21 @@
       <c r="C90" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D90" s="5"/>
+      <c r="D90" s="7"/>
     </row>
     <row r="91" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="7" t="s">
         <v>157</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>158</v>
       </c>
       <c r="D91" s="3"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
@@ -1936,7 +1825,7 @@
       <c r="D93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="11" t="s">
         <v>164</v>
       </c>
       <c r="B94" s="3"/>
@@ -1944,12 +1833,12 @@
       <c r="E94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="10" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="10" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1963,13 +1852,13 @@
       <c r="C97" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="D97" s="5"/>
+      <c r="D97" s="7"/>
     </row>
     <row r="98" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="7" t="s">
         <v>171</v>
       </c>
       <c r="C98" s="6" t="s">

</xml_diff>